<commit_message>
classified files and code in different folders
</commit_message>
<xml_diff>
--- a/excel/NIS Phone Case Photos URL.xlsx
+++ b/excel/NIS Phone Case Photos URL.xlsx
@@ -458,594 +458,594 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23 Ultra_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23%20Ultra_01.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23 Ultra_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23%20Ultra_02.jpg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23 Ultra_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23%20Ultra_Features.jpg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23 Ultra_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23%20Ultra_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23+_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23+_01.jpg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23+_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23+_02.jpg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23+_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23+_Features.jpg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S23+_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S23+_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24 Ultra_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24%20Ultra_01.jpg</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24 Ultra_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24%20Ultra_02.jpg</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24 Ultra_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24%20Ultra_Features.jpg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24 Ultra_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24%20Ultra_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24+_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24+_01.jpg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24+_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24+_02.jpg</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24+_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24+_Features.jpg</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_Samsung Galaxy S24+_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_Samsung%20Galaxy%20S24+_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14 Pro_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014%20Pro_01.jpg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14 Pro_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014%20Pro_02.jpg</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14 Pro_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014%20Pro_Features.jpg</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14 Pro_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014%20Pro_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014_01.jpg</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014_02.jpg</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014_Features.jpg</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 14_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2014_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro Max_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro%20Max_01.jpg</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro Max_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro%20Max_02.jpg</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro Max_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro%20Max_Features.jpg</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro Max_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro%20Max_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro_01.jpg</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro_02.jpg</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro_Features.jpg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15 Pro_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015%20Pro_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015_01.jpg</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015_02.jpg</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015_Features.jpg</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night Over the Rhône_iPhone 15_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night%20Over%20the%20Rhône_iPhone%2015_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23 Ultra_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23%20Ultra_01.jpg</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23 Ultra_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23%20Ultra_02.jpg</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23 Ultra_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23%20Ultra_Features.jpg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23 Ultra_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23%20Ultra_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23+_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23+_01.jpg</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23+_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23+_02.jpg</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23+_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23+_Features.jpg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S23+_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S23+_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24 Ultra_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24%20Ultra_01.jpg</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24 Ultra_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24%20Ultra_02.jpg</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24 Ultra_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24%20Ultra_Features.jpg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24 Ultra_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24%20Ultra_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24+_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24+_01.jpg</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24+_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24+_02.jpg</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24+_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24+_Features.jpg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_Samsung Galaxy S24+_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_Samsung%20Galaxy%20S24+_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14 Pro_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014%20Pro_01.jpg</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14 Pro_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014%20Pro_02.jpg</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14 Pro_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014%20Pro_Features.jpg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14 Pro_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014%20Pro_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014_01.jpg</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014_02.jpg</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014_Features.jpg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 14_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2014_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro Max_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro%20Max_01.jpg</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro Max_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro%20Max_02.jpg</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro Max_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro%20Max_Features.jpg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro Max_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro%20Max_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro_01.jpg</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro_02.jpg</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro_Features.jpg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15 Pro_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015%20Pro_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015_01.jpg</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015_02.jpg</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015_Features.jpg</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry Night_iPhone 15_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Starry%20Night_iPhone%2015_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23 Ultra_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23%20Ultra_01.jpg</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23 Ultra_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23%20Ultra_02.jpg</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23 Ultra_Fratures.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23%20Ultra_Fratures.jpg</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23 Ultra_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23%20Ultra_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23+_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23+_01.jpg</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23+_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23+_02.jpg</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23+_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23+_Features.jpg</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S23+_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S23+_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24 Ultra_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24%20Ultra_01.jpg</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24 Ultra_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24%20Ultra_02.jpg</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24 Ultra_Fratures.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24%20Ultra_Fratures.jpg</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24 Ultra_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24%20Ultra_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24+_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24+_01.jpg</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24+_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24+_02.jpg</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24+_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24+_Features.jpg</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_Samsung Galaxy S24+_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_Samsung%20Galaxy%20S24+_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14 Pro_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014%20Pro_01.jpg</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14 Pro_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014%20Pro_02.jpg</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14 Pro_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014%20Pro_Features.jpg</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14 Pro_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014%20Pro_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014_01.jpg</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014_02.jpg</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014_Features.jpg</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 14_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2014_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro Max_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro%20Max_01.jpg</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro Max_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro%20Max_02.jpg</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro Max_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro%20Max_Features.jpg</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro Max_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro%20Max_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro_01.jpg</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro_02.jpg</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro_Features.jpg</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15 Pro_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015%20Pro_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15_01.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015_01.jpg</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15_02.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015_02.jpg</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15_Features.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015_Features.jpg</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise Impression_iPhone 15_Light and Thin.jpg</t>
+          <t>https://raw.githubusercontent.com/SageCat/noon-images/main/images/noon/PhoneCase/Sunrise%20Impression_iPhone%2015_Light%20and%20Thin.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>